<commit_message>
Updated as on 7th Feb
</commit_message>
<xml_diff>
--- a/POMFramework_Sarathi/DataFiles/Services.xlsx
+++ b/POMFramework_Sarathi/DataFiles/Services.xlsx
@@ -3687,10 +3687,10 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>UP90120100000768</t>
-  </si>
-  <si>
-    <t>343721</t>
+    <t>OD90120100000022</t>
+  </si>
+  <si>
+    <t>353021</t>
   </si>
 </sst>
 </file>
@@ -4331,8 +4331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B15"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4470,10 +4470,10 @@
         <v>CAS_SarathiCOV</v>
       </c>
       <c r="F2" s="63" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G2" s="63" t="s">
-        <v>801</v>
+        <v>498</v>
       </c>
       <c r="H2" s="48" t="s">
         <v>864</v>
@@ -4481,8 +4481,8 @@
       <c r="I2" s="48" t="s">
         <v>864</v>
       </c>
-      <c r="J2" s="82" t="s">
-        <v>873</v>
+      <c r="J2" s="85" t="s">
+        <v>869</v>
       </c>
       <c r="K2" s="47" t="str">
         <f>VLOOKUP(J:J,MasterData!I1:J39,2,FALSE)</f>

</xml_diff>